<commit_message>
Update months for sheet 1 in the letaba data collection
</commit_message>
<xml_diff>
--- a/data/WLE project 2021-11-15 Letaba_EWR4 NAT.xlsx
+++ b/data/WLE project 2021-11-15 Letaba_EWR4 NAT.xlsx
@@ -1,31 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vuyisile\Desktop\Letaba\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corywhitney/Dropbox/Contributions/21_WLE_Letaba/Limpopo_model/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D807BC59-3B70-8144-9B0C-4302C7EF2620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6750"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34020" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LET2 nat" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t>Oct</t>
   </si>
@@ -99,7 +107,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -209,7 +217,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -280,40 +288,40 @@
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dec</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Jan</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>Feb</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>Mar</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>Apr</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>May</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>Jun</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>Jul</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>Aug</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>Sep</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Oct</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Nov</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Dec</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -387,40 +395,40 @@
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dec</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Jan</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>Feb</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>Mar</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>Apr</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>May</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>Jun</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>Jul</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>Aug</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>Sep</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Oct</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Nov</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Dec</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -494,40 +502,40 @@
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dec</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Jan</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>Feb</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>Mar</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>Apr</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>May</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>Jun</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>Jul</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>Aug</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>Sep</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Oct</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Nov</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Dec</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -601,40 +609,40 @@
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dec</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Jan</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>Feb</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>Mar</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>Apr</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>May</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>Jun</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>Jul</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>Aug</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>Sep</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Oct</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Nov</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Dec</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -708,40 +716,40 @@
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dec</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Jan</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>Feb</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>Mar</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>Apr</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>May</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>Jun</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>Jul</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>Aug</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>Sep</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Oct</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Nov</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Dec</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2563,7 +2571,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0955146-02D4-4A41-A73B-448CF885A52B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2601,7 +2609,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0955146-02D4-4A41-A73B-448CF885A52B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2639,7 +2647,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0955146-02D4-4A41-A73B-448CF885A52B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2924,27 +2932,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:AB150"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="293" zoomScaleNormal="293" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="5.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
@@ -2957,7 +2963,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -2999,7 +3005,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1920</v>
       </c>
@@ -3095,7 +3101,7 @@
         <v>490.10000000000008</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1921</v>
       </c>
@@ -3191,7 +3197,7 @@
         <v>256.08000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1922</v>
       </c>
@@ -3287,7 +3293,7 @@
         <v>1487.9899999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1923</v>
       </c>
@@ -3383,7 +3389,7 @@
         <v>344.93000000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1924</v>
       </c>
@@ -3479,7 +3485,7 @@
         <v>1419.2</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1925</v>
       </c>
@@ -3575,7 +3581,7 @@
         <v>203.77999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1926</v>
       </c>
@@ -3671,7 +3677,7 @@
         <v>136.05000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1927</v>
       </c>
@@ -3767,7 +3773,7 @@
         <v>276.12000000000006</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1928</v>
       </c>
@@ -3863,7 +3869,7 @@
         <v>322.86</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>1929</v>
       </c>
@@ -3959,7 +3965,7 @@
         <v>333.91</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>1930</v>
       </c>
@@ -4055,7 +4061,7 @@
         <v>479.13</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>1931</v>
       </c>
@@ -4151,7 +4157,7 @@
         <v>200.4</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>1932</v>
       </c>
@@ -4247,7 +4253,7 @@
         <v>326.35000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>1933</v>
       </c>
@@ -4343,7 +4349,7 @@
         <v>454.60999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>1934</v>
       </c>
@@ -4439,7 +4445,7 @@
         <v>221.04999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>1935</v>
       </c>
@@ -4535,7 +4541,7 @@
         <v>235.14000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>1936</v>
       </c>
@@ -4631,7 +4637,7 @@
         <v>991.53</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>1937</v>
       </c>
@@ -4727,7 +4733,7 @@
         <v>319.39999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>1938</v>
       </c>
@@ -4823,7 +4829,7 @@
         <v>1166.3499999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>1939</v>
       </c>
@@ -4919,7 +4925,7 @@
         <v>388.46</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>1940</v>
       </c>
@@ -5015,7 +5021,7 @@
         <v>213.42</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>1941</v>
       </c>
@@ -5111,7 +5117,7 @@
         <v>296.53999999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>1942</v>
       </c>
@@ -5207,7 +5213,7 @@
         <v>337.09999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>1943</v>
       </c>
@@ -5303,7 +5309,7 @@
         <v>323.35000000000008</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>1944</v>
       </c>
@@ -5399,7 +5405,7 @@
         <v>270.51</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>1945</v>
       </c>
@@ -5495,7 +5501,7 @@
         <v>495.60000000000008</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>1946</v>
       </c>
@@ -5591,7 +5597,7 @@
         <v>169.26</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>1947</v>
       </c>
@@ -5687,7 +5693,7 @@
         <v>604.77</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>1948</v>
       </c>
@@ -5783,7 +5789,7 @@
         <v>276.32000000000005</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>1949</v>
       </c>
@@ -5879,7 +5885,7 @@
         <v>288.71999999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>1950</v>
       </c>
@@ -5975,7 +5981,7 @@
         <v>273.28000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>1951</v>
       </c>
@@ -6071,7 +6077,7 @@
         <v>132.76999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>1952</v>
       </c>
@@ -6167,7 +6173,7 @@
         <v>552.86</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>1953</v>
       </c>
@@ -6263,7 +6269,7 @@
         <v>348.50999999999988</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>1954</v>
       </c>
@@ -6359,7 +6365,7 @@
         <v>744.62</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>1955</v>
       </c>
@@ -6455,7 +6461,7 @@
         <v>893.32999999999993</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>1956</v>
       </c>
@@ -6551,7 +6557,7 @@
         <v>242.70999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>1957</v>
       </c>
@@ -6647,7 +6653,7 @@
         <v>1080.53</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>1958</v>
       </c>
@@ -6743,7 +6749,7 @@
         <v>321.33</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>1959</v>
       </c>
@@ -6839,7 +6845,7 @@
         <v>315.87999999999994</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>1960</v>
       </c>
@@ -6935,7 +6941,7 @@
         <v>581.18999999999994</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>1961</v>
       </c>
@@ -7031,7 +7037,7 @@
         <v>151.41</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>1962</v>
       </c>
@@ -7127,7 +7133,7 @@
         <v>195.04000000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>1963</v>
       </c>
@@ -7223,7 +7229,7 @@
         <v>127.99000000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>1964</v>
       </c>
@@ -7319,7 +7325,7 @@
         <v>341.88999999999993</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>1965</v>
       </c>
@@ -7415,7 +7421,7 @@
         <v>215.14999999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>1966</v>
       </c>
@@ -7511,7 +7517,7 @@
         <v>559.61</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>1967</v>
       </c>
@@ -7607,7 +7613,7 @@
         <v>150.07999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>1968</v>
       </c>
@@ -7703,7 +7709,7 @@
         <v>401.15999999999991</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>1969</v>
       </c>
@@ -7799,7 +7805,7 @@
         <v>155.42000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>1970</v>
       </c>
@@ -7895,7 +7901,7 @@
         <v>224.02</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>1971</v>
       </c>
@@ -7991,7 +7997,7 @@
         <v>1045.7900000000002</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>1972</v>
       </c>
@@ -8087,7 +8093,7 @@
         <v>169.60000000000002</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>1973</v>
       </c>
@@ -8183,7 +8189,7 @@
         <v>901.06999999999982</v>
       </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>1974</v>
       </c>
@@ -8279,7 +8285,7 @@
         <v>489.75</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>1975</v>
       </c>
@@ -8375,7 +8381,7 @@
         <v>793.2199999999998</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>1976</v>
       </c>
@@ -8471,7 +8477,7 @@
         <v>565.59999999999991</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>1977</v>
       </c>
@@ -8567,7 +8573,7 @@
         <v>656.15</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>1978</v>
       </c>
@@ -8663,7 +8669,7 @@
         <v>199.82999999999998</v>
       </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>1979</v>
       </c>
@@ -8759,7 +8765,7 @@
         <v>606.92999999999995</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>1980</v>
       </c>
@@ -8855,7 +8861,7 @@
         <v>926.21</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>1981</v>
       </c>
@@ -8951,7 +8957,7 @@
         <v>152.47000000000003</v>
       </c>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>1982</v>
       </c>
@@ -9047,7 +9053,7 @@
         <v>95.340000000000018</v>
       </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>1983</v>
       </c>
@@ -9143,7 +9149,7 @@
         <v>156.02000000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>1984</v>
       </c>
@@ -9239,7 +9245,7 @@
         <v>298.16999999999996</v>
       </c>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>1985</v>
       </c>
@@ -9335,7 +9341,7 @@
         <v>243.87</v>
       </c>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>1986</v>
       </c>
@@ -9431,7 +9437,7 @@
         <v>228.04000000000002</v>
       </c>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>1987</v>
       </c>
@@ -9527,7 +9533,7 @@
         <v>617.65</v>
       </c>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>1988</v>
       </c>
@@ -9623,7 +9629,7 @@
         <v>201.1</v>
       </c>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>1989</v>
       </c>
@@ -9719,7 +9725,7 @@
         <v>275.14000000000004</v>
       </c>
     </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>1990</v>
       </c>
@@ -9815,7 +9821,7 @@
         <v>381.88</v>
       </c>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A74">
         <v>1991</v>
       </c>
@@ -9911,7 +9917,7 @@
         <v>87.37</v>
       </c>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A75">
         <v>1992</v>
       </c>
@@ -10007,7 +10013,7 @@
         <v>144.61000000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A76">
         <v>1993</v>
       </c>
@@ -10103,7 +10109,7 @@
         <v>164.07</v>
       </c>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A77">
         <v>1994</v>
       </c>
@@ -10199,7 +10205,7 @@
         <v>189.41000000000003</v>
       </c>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A78">
         <v>1995</v>
       </c>
@@ -10295,7 +10301,7 @@
         <v>1195.81</v>
       </c>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A79">
         <v>1996</v>
       </c>
@@ -10391,7 +10397,7 @@
         <v>557.12999999999988</v>
       </c>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A80">
         <v>1997</v>
       </c>
@@ -10487,7 +10493,7 @@
         <v>235.85</v>
       </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A81">
         <v>1998</v>
       </c>
@@ -10583,7 +10589,7 @@
         <v>580.86</v>
       </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A82">
         <v>1999</v>
       </c>
@@ -10679,7 +10685,7 @@
         <v>3423.2099999999996</v>
       </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A83">
         <v>2000</v>
       </c>
@@ -10775,7 +10781,7 @@
         <v>387.57</v>
       </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A84">
         <v>2001</v>
       </c>
@@ -10871,7 +10877,7 @@
         <v>296.85000000000002</v>
       </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A85">
         <v>2002</v>
       </c>
@@ -10967,7 +10973,7 @@
         <v>78.78</v>
       </c>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A86">
         <v>2003</v>
       </c>
@@ -11063,7 +11069,7 @@
         <v>461.36</v>
       </c>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A87">
         <v>2004</v>
       </c>
@@ -11159,7 +11165,7 @@
         <v>140.82</v>
       </c>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A88">
         <v>2005</v>
       </c>
@@ -11255,7 +11261,7 @@
         <v>452.13000000000005</v>
       </c>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A89">
         <v>2006</v>
       </c>
@@ -11351,7 +11357,7 @@
         <v>137.66</v>
       </c>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A90" s="1">
         <v>2007</v>
       </c>
@@ -11447,7 +11453,7 @@
         <v>254.23</v>
       </c>
     </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A91" s="1">
         <v>2008</v>
       </c>
@@ -11543,7 +11549,7 @@
         <v>274.53000000000003</v>
       </c>
     </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A92" s="1">
         <v>2009</v>
       </c>
@@ -11639,7 +11645,7 @@
         <v>333.35</v>
       </c>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A93" s="1">
         <v>2010</v>
       </c>
@@ -11735,7 +11741,7 @@
         <v>429.07999999999993</v>
       </c>
     </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
         <v>13</v>
       </c>
@@ -11843,7 +11849,7 @@
         <v>450.4157647058824</v>
       </c>
     </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A95" s="1" t="s">
         <v>14</v>
       </c>
@@ -11896,7 +11902,7 @@
         <v>1.3850308641975306</v>
       </c>
     </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A96" s="1" t="s">
         <v>15</v>
       </c>
@@ -11949,7 +11955,7 @@
         <v>7.4575617283950617</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A97" s="1" t="s">
         <v>16</v>
       </c>
@@ -11990,7 +11996,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A98" s="10">
         <v>0.1</v>
       </c>
@@ -12043,7 +12049,7 @@
         <v>7.4433256172839499</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A99" s="10">
         <v>1</v>
       </c>
@@ -12096,7 +12102,7 @@
         <v>7.3152006172839501</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A100" s="10">
         <v>5</v>
       </c>
@@ -12149,7 +12155,7 @@
         <v>6.1207561728395055</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A101" s="10">
         <v>10</v>
       </c>
@@ -12202,7 +12208,7 @@
         <v>5.6597222222222223</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A102" s="10">
         <v>15</v>
       </c>
@@ -12255,7 +12261,7 @@
         <v>5.3973765432098766</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A103" s="10">
         <v>20</v>
       </c>
@@ -12308,7 +12314,7 @@
         <v>5.0154320987654319</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A104" s="10">
         <v>30</v>
       </c>
@@ -12361,7 +12367,7 @@
         <v>4.710648148148147</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A105" s="10">
         <v>40</v>
       </c>
@@ -12414,7 +12420,7 @@
         <v>4.3981481481481479</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A106" s="10">
         <v>50</v>
       </c>
@@ -12467,7 +12473,7 @@
         <v>4.0856481481481479</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A107" s="10">
         <v>60</v>
       </c>
@@ -12520,7 +12526,7 @@
         <v>3.4876543209876538</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A108" s="10">
         <v>70</v>
       </c>
@@ -12573,7 +12579,7 @@
         <v>3.2060185185185186</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A109" s="10">
         <v>80</v>
       </c>
@@ -12626,7 +12632,7 @@
         <v>2.7662037037037037</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A110" s="10">
         <v>85</v>
       </c>
@@ -12679,7 +12685,7 @@
         <v>2.6157407407407405</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A111" s="10">
         <v>90</v>
       </c>
@@ -12732,7 +12738,7 @@
         <v>2.492283950617284</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A112" s="10">
         <v>95</v>
       </c>
@@ -12785,7 +12791,7 @@
         <v>2.0756172839506171</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A113" s="10">
         <v>99</v>
       </c>
@@ -12838,7 +12844,7 @@
         <v>1.5551697530864197</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A114" s="10">
         <v>99.9</v>
       </c>
@@ -12891,52 +12897,64 @@
         <v>1.4020447530864195</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A115" s="12"/>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A116" s="12"/>
     </row>
-    <row r="117" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A117" s="15"/>
-      <c r="B117" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C117" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D117" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E117" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F117" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="G117" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H117" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I117" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J117" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="K117" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="L117" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M117" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B117" s="15" t="str">
+        <f>B97</f>
+        <v>Oct</v>
+      </c>
+      <c r="C117" s="15" t="str">
+        <f t="shared" ref="C117:M117" si="45">C97</f>
+        <v>Nov</v>
+      </c>
+      <c r="D117" s="15" t="str">
+        <f t="shared" si="45"/>
+        <v>Dec</v>
+      </c>
+      <c r="E117" s="15" t="str">
+        <f t="shared" si="45"/>
+        <v>Jan</v>
+      </c>
+      <c r="F117" s="15" t="str">
+        <f t="shared" si="45"/>
+        <v>Feb</v>
+      </c>
+      <c r="G117" s="15" t="str">
+        <f t="shared" si="45"/>
+        <v>Mar</v>
+      </c>
+      <c r="H117" s="15" t="str">
+        <f t="shared" si="45"/>
+        <v>Apr</v>
+      </c>
+      <c r="I117" s="15" t="str">
+        <f t="shared" si="45"/>
+        <v>May</v>
+      </c>
+      <c r="J117" s="15" t="str">
+        <f t="shared" si="45"/>
+        <v>Jun</v>
+      </c>
+      <c r="K117" s="15" t="str">
+        <f t="shared" si="45"/>
+        <v>Jul</v>
+      </c>
+      <c r="L117" s="15" t="str">
+        <f t="shared" si="45"/>
+        <v>Aug</v>
+      </c>
+      <c r="M117" s="15" t="str">
+        <f t="shared" si="45"/>
+        <v>Sep</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A118" s="16" t="s">
         <v>21</v>
       </c>
@@ -12945,51 +12963,51 @@
         <v>5.2942054958183995</v>
       </c>
       <c r="C118" s="17">
-        <f t="shared" ref="C118:M118" si="45">C102</f>
+        <f t="shared" ref="C118:M118" si="46">C102</f>
         <v>9.1319444444444446</v>
       </c>
       <c r="D118" s="17">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>17.803539426523297</v>
       </c>
       <c r="E118" s="17">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>40.725806451612904</v>
       </c>
       <c r="F118" s="17">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>81.696574893477546</v>
       </c>
       <c r="G118" s="17">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>57.246863799283155</v>
       </c>
       <c r="H118" s="17">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>25.152391975308639</v>
       </c>
       <c r="I118" s="17">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>12.589605734767023</v>
       </c>
       <c r="J118" s="17">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>8.3912037037037024</v>
       </c>
       <c r="K118" s="17">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>6.5804211469534044</v>
       </c>
       <c r="L118" s="17">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>5.7646356033452806</v>
       </c>
       <c r="M118" s="17">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>5.3973765432098766</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A119" s="16" t="s">
         <v>18</v>
       </c>
@@ -12998,51 +13016,51 @@
         <v>8.400052270011944</v>
       </c>
       <c r="C119" s="17">
-        <f t="shared" ref="C119:M119" si="46">C98</f>
+        <f t="shared" ref="C119:M119" si="47">C98</f>
         <v>30.926427469135767</v>
       </c>
       <c r="D119" s="17">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>71.782295400238908</v>
       </c>
       <c r="E119" s="17">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>219.01239545997572</v>
       </c>
       <c r="F119" s="17">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>593.02671255326004</v>
       </c>
       <c r="G119" s="17">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>450.95202359617599</v>
       </c>
       <c r="H119" s="17">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>137.87642746913571</v>
       </c>
       <c r="I119" s="17">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>21.562499999999989</v>
       </c>
       <c r="J119" s="17">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>11.425810185185185</v>
       </c>
       <c r="K119" s="17">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>9.6364620669056098</v>
       </c>
       <c r="L119" s="17">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>8.76530764635603</v>
       </c>
       <c r="M119" s="17">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>7.4433256172839499</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A120" s="16" t="s">
         <v>19</v>
       </c>
@@ -13051,51 +13069,51 @@
         <v>3.7335722819593791</v>
       </c>
       <c r="C120" s="17">
-        <f t="shared" ref="C120:M120" si="47">C106</f>
+        <f t="shared" ref="C120:M120" si="48">C106</f>
         <v>5.3317901234567904</v>
       </c>
       <c r="D120" s="17">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>9.240591397849462</v>
       </c>
       <c r="E120" s="17">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>12.865890083632017</v>
       </c>
       <c r="F120" s="17">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>17.79334644378892</v>
       </c>
       <c r="G120" s="17">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>14.859617682198326</v>
       </c>
       <c r="H120" s="17">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>11.797839506172838</v>
       </c>
       <c r="I120" s="17">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>7.5791517323775386</v>
       </c>
       <c r="J120" s="17">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>6.1959876543209873</v>
       </c>
       <c r="K120" s="17">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>5.1299283154121857</v>
       </c>
       <c r="L120" s="17">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>4.6258960573476697</v>
       </c>
       <c r="M120" s="17">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>4.0856481481481479</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A121" s="16" t="s">
         <v>20</v>
       </c>
@@ -13104,51 +13122,51 @@
         <v>1.2598939665471924</v>
       </c>
       <c r="C121" s="17">
-        <f t="shared" ref="C121:M121" si="48">C114</f>
+        <f t="shared" ref="C121:M121" si="49">C114</f>
         <v>1.3709490740740742</v>
       </c>
       <c r="D121" s="17">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>1.8733572281959379</v>
       </c>
       <c r="E121" s="17">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>2.8658154121863801</v>
       </c>
       <c r="F121" s="17">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>3.1529006882989181</v>
       </c>
       <c r="G121" s="17">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>3.2857676224611705</v>
       </c>
       <c r="H121" s="17">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>3.1644290123456789</v>
       </c>
       <c r="I121" s="17">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>2.3671968339307052</v>
       </c>
       <c r="J121" s="17">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>2.1442515432098768</v>
       </c>
       <c r="K121" s="17">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>1.81432945041816</v>
       </c>
       <c r="L121" s="17">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>1.5907631421744326</v>
       </c>
       <c r="M121" s="17">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>1.4020447530864195</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A122" s="16" t="s">
         <v>22</v>
       </c>
@@ -13157,63 +13175,63 @@
         <v>2.4436230585424132</v>
       </c>
       <c r="C122" s="17">
-        <f t="shared" ref="C122:M122" si="49">C110</f>
+        <f t="shared" ref="C122:M122" si="50">C110</f>
         <v>3.0748456790123457</v>
       </c>
       <c r="D122" s="17">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>4.2506720430107521</v>
       </c>
       <c r="E122" s="17">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>6.397476105137395</v>
       </c>
       <c r="F122" s="17">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>7.3111274991805963</v>
       </c>
       <c r="G122" s="17">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>6.0633213859020305</v>
       </c>
       <c r="H122" s="17">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>5.6886574074074074</v>
       </c>
       <c r="I122" s="17">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>4.8704450418160086</v>
       </c>
       <c r="J122" s="17">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>4.2033179012345681</v>
       </c>
       <c r="K122" s="17">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>3.5375597371565108</v>
       </c>
       <c r="L122" s="17">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>3.0167264038231787</v>
       </c>
       <c r="M122" s="17">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>2.6157407407407405</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A123" s="12"/>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A124" s="6"/>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A128" s="6"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A143" s="6"/>
     </row>
-    <row r="145" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A145" s="15"/>
       <c r="B145" s="15" t="s">
         <v>3</v>
@@ -13252,7 +13270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A146" s="16">
         <v>1999</v>
       </c>
@@ -13294,7 +13312,7 @@
       </c>
       <c r="N146" s="8"/>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A147" s="16">
         <v>1938</v>
       </c>
@@ -13336,7 +13354,7 @@
       </c>
       <c r="N147" s="8"/>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A148" s="16">
         <v>1951</v>
       </c>
@@ -13378,7 +13396,7 @@
       </c>
       <c r="N148" s="8"/>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A149" s="16">
         <v>1991</v>
       </c>
@@ -13420,7 +13438,7 @@
       </c>
       <c r="N149" s="8"/>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A150" s="16">
         <v>2002</v>
       </c>
@@ -13507,16 +13525,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N91"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:M91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1">
         <v>1920</v>
       </c>
@@ -13560,7 +13578,7 @@
         <v>490.12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1921</v>
       </c>
@@ -13604,7 +13622,7 @@
         <v>256.11</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1922</v>
       </c>
@@ -13648,7 +13666,7 @@
         <v>1488.01</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1923</v>
       </c>
@@ -13692,7 +13710,7 @@
         <v>344.95</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1924</v>
       </c>
@@ -13736,7 +13754,7 @@
         <v>1419.21</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1925</v>
       </c>
@@ -13780,7 +13798,7 @@
         <v>203.8</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1926</v>
       </c>
@@ -13824,7 +13842,7 @@
         <v>136.07</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1927</v>
       </c>
@@ -13868,7 +13886,7 @@
         <v>276.13</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1928</v>
       </c>
@@ -13912,7 +13930,7 @@
         <v>322.88</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1929</v>
       </c>
@@ -13956,7 +13974,7 @@
         <v>333.92</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1930</v>
       </c>
@@ -14000,7 +14018,7 @@
         <v>479.15</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>1931</v>
       </c>
@@ -14044,7 +14062,7 @@
         <v>200.43</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>1932</v>
       </c>
@@ -14088,7 +14106,7 @@
         <v>326.36</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>1933</v>
       </c>
@@ -14132,7 +14150,7 @@
         <v>454.62</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>1934</v>
       </c>
@@ -14176,7 +14194,7 @@
         <v>221.06</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>1935</v>
       </c>
@@ -14220,7 +14238,7 @@
         <v>235.15</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>1936</v>
       </c>
@@ -14264,7 +14282,7 @@
         <v>991.54</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>1937</v>
       </c>
@@ -14308,7 +14326,7 @@
         <v>319.41000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>1938</v>
       </c>
@@ -14352,7 +14370,7 @@
         <v>1166.3900000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>1939</v>
       </c>
@@ -14396,7 +14414,7 @@
         <v>388.47</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>1940</v>
       </c>
@@ -14440,7 +14458,7 @@
         <v>213.44</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>1941</v>
       </c>
@@ -14484,7 +14502,7 @@
         <v>296.55</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>1942</v>
       </c>
@@ -14528,7 +14546,7 @@
         <v>337.12</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>1943</v>
       </c>
@@ -14572,7 +14590,7 @@
         <v>323.36</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>1944</v>
       </c>
@@ -14616,7 +14634,7 @@
         <v>270.52</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>1945</v>
       </c>
@@ -14660,7 +14678,7 @@
         <v>495.61</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>1946</v>
       </c>
@@ -14704,7 +14722,7 @@
         <v>169.26</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>1947</v>
       </c>
@@ -14748,7 +14766,7 @@
         <v>604.79999999999995</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>1948</v>
       </c>
@@ -14792,7 +14810,7 @@
         <v>276.33999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>1949</v>
       </c>
@@ -14836,7 +14854,7 @@
         <v>288.72000000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>1950</v>
       </c>
@@ -14880,7 +14898,7 @@
         <v>273.3</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>1951</v>
       </c>
@@ -14924,7 +14942,7 @@
         <v>132.79</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>1952</v>
       </c>
@@ -14968,7 +14986,7 @@
         <v>552.87</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>1953</v>
       </c>
@@ -15012,7 +15030,7 @@
         <v>348.52</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>1954</v>
       </c>
@@ -15056,7 +15074,7 @@
         <v>744.65</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>1955</v>
       </c>
@@ -15100,7 +15118,7 @@
         <v>893.34</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>1956</v>
       </c>
@@ -15144,7 +15162,7 @@
         <v>242.74</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>1957</v>
       </c>
@@ -15188,7 +15206,7 @@
         <v>1080.54</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>1958</v>
       </c>
@@ -15232,7 +15250,7 @@
         <v>321.33999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>1959</v>
       </c>
@@ -15276,7 +15294,7 @@
         <v>315.91000000000003</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>1960</v>
       </c>
@@ -15320,7 +15338,7 @@
         <v>581.21</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>1961</v>
       </c>
@@ -15364,7 +15382,7 @@
         <v>151.43</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>1962</v>
       </c>
@@ -15408,7 +15426,7 @@
         <v>195.06</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>1963</v>
       </c>
@@ -15452,7 +15470,7 @@
         <v>128.01</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>1964</v>
       </c>
@@ -15496,7 +15514,7 @@
         <v>341.91</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>1965</v>
       </c>
@@ -15540,7 +15558,7 @@
         <v>215.17</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>1966</v>
       </c>
@@ -15584,7 +15602,7 @@
         <v>559.62</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>1967</v>
       </c>
@@ -15628,7 +15646,7 @@
         <v>150.1</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>1968</v>
       </c>
@@ -15672,7 +15690,7 @@
         <v>401.18</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>1969</v>
       </c>
@@ -15716,7 +15734,7 @@
         <v>155.44</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>1970</v>
       </c>
@@ -15760,7 +15778,7 @@
         <v>224.03</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>1971</v>
       </c>
@@ -15804,7 +15822,7 @@
         <v>1045.82</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>1972</v>
       </c>
@@ -15848,7 +15866,7 @@
         <v>169.63</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>1973</v>
       </c>
@@ -15892,7 +15910,7 @@
         <v>901.08</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>1974</v>
       </c>
@@ -15936,7 +15954,7 @@
         <v>489.77</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>1975</v>
       </c>
@@ -15980,7 +15998,7 @@
         <v>793.23</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>1976</v>
       </c>
@@ -16024,7 +16042,7 @@
         <v>565.62</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>1977</v>
       </c>
@@ -16068,7 +16086,7 @@
         <v>656.17</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>1978</v>
       </c>
@@ -16112,7 +16130,7 @@
         <v>199.86</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>1979</v>
       </c>
@@ -16156,7 +16174,7 @@
         <v>606.92999999999995</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>1980</v>
       </c>
@@ -16200,7 +16218,7 @@
         <v>926.23</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>1981</v>
       </c>
@@ -16244,7 +16262,7 @@
         <v>152.49</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>1982</v>
       </c>
@@ -16288,7 +16306,7 @@
         <v>95.35</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>1983</v>
       </c>
@@ -16332,7 +16350,7 @@
         <v>156.03</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>1984</v>
       </c>
@@ -16376,7 +16394,7 @@
         <v>298.18</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>1985</v>
       </c>
@@ -16420,7 +16438,7 @@
         <v>243.89</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>1986</v>
       </c>
@@ -16464,7 +16482,7 @@
         <v>228.06</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>1987</v>
       </c>
@@ -16508,7 +16526,7 @@
         <v>617.66999999999996</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>1988</v>
       </c>
@@ -16552,7 +16570,7 @@
         <v>201.13</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>1989</v>
       </c>
@@ -16596,7 +16614,7 @@
         <v>275.14</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>1990</v>
       </c>
@@ -16640,7 +16658,7 @@
         <v>381.89</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>1991</v>
       </c>
@@ -16684,7 +16702,7 @@
         <v>87.38</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>1992</v>
       </c>
@@ -16728,7 +16746,7 @@
         <v>144.62</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A74">
         <v>1993</v>
       </c>
@@ -16772,7 +16790,7 @@
         <v>164.09</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A75">
         <v>1994</v>
       </c>
@@ -16816,7 +16834,7 @@
         <v>189.43</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A76">
         <v>1995</v>
       </c>
@@ -16860,7 +16878,7 @@
         <v>1195.81</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A77">
         <v>1996</v>
       </c>
@@ -16904,7 +16922,7 @@
         <v>557.15</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A78">
         <v>1997</v>
       </c>
@@ -16948,7 +16966,7 @@
         <v>235.87</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A79">
         <v>1998</v>
       </c>
@@ -16992,7 +17010,7 @@
         <v>580.87</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A80">
         <v>1999</v>
       </c>
@@ -17036,7 +17054,7 @@
         <v>3423.22</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A81">
         <v>2000</v>
       </c>
@@ -17080,7 +17098,7 @@
         <v>387.58</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A82">
         <v>2001</v>
       </c>
@@ -17124,7 +17142,7 @@
         <v>296.87</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A83">
         <v>2002</v>
       </c>
@@ -17168,7 +17186,7 @@
         <v>78.790000000000006</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A84">
         <v>2003</v>
       </c>
@@ -17212,7 +17230,7 @@
         <v>461.37</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A85">
         <v>2004</v>
       </c>
@@ -17256,7 +17274,7 @@
         <v>140.84</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A86">
         <v>2005</v>
       </c>
@@ -17300,7 +17318,7 @@
         <v>452.14</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A87">
         <v>2006</v>
       </c>
@@ -17344,7 +17362,7 @@
         <v>137.68</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A88">
         <v>2007</v>
       </c>
@@ -17388,7 +17406,7 @@
         <v>254.24</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A89">
         <v>2008</v>
       </c>
@@ -17432,7 +17450,7 @@
         <v>274.55</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A90">
         <v>2009</v>
       </c>
@@ -17476,7 +17494,7 @@
         <v>333.37</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A91">
         <v>2010</v>
       </c>

</xml_diff>